<commit_message>
Ajout d'un invariant INS pour envoyer un warning quand on a un code COG 99999 dans le cadre d'une identité validée (#262)
* add invariant

* update

* update

* ajout de la ligne dans le changelog 641b05582748be1db5916dfad5e730858b42e887
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-core-patient-ins.xlsx
+++ b/main/ig/StructureDefinition-fr-core-patient-ins.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-21T08:47:55+00:00</t>
+    <t>2026-01-28T09:35:28+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -88,7 +88,7 @@
   </si>
   <si>
     <t>FR Core Patient profile overspecified to comply with the requirements of the National Health Identity (INS) framework. The INS identifier can only be conveyed in the case of a qualified identity, which is why the identifier slices are defined in the FRCorePatientINS profile and not in the FRCorePatient profile.
-Profil Fr Core Patient surspécifié pour être conforme aux exigences du référentiel d'Identité Nationale de Santé (INS). Le matricule INS ne peut être véhiculé que dans le cas d'une identité qualifiée, raison pour laquelle les slices identifier sont définies au niveau du FRCorePatientINS et non au niveau du FRCorePatient.</t>
+Profil FR Core Patient surspécifié pour être conforme aux exigences du référentiel d'Identité Nationale de Santé (INS). Le matricule INS ne peut être véhiculé que dans le cas d'une identité qualifiée, raison pour laquelle les slices identifier sont définies au niveau du FRCorePatientINS et non au niveau du FRCorePatient.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -280,7 +280,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}fr-core-1:If identityReliability status = 'VALI', then at least Patient.identifier[INS-NIR] or Patient.identifier[INS-NIA] or Patient.identifier[INS-NIR-TEST] or Patient.identifier[INS-NIR-DEMO] SHALL be present {(extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-identity-reliability').extension('identityStatus').value.exists(code = 'VALI')) implies (identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.8' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.9' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.10' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.11' and use = 'official').exists())}fr-core-2:If identityReliability status = 'VALI', then only one identifier of type official SHALL be present {(extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-identity-reliability').extension('identityStatus').value.exists(code = 'VALI')) implies (identifier.where(use = 'official').count() = 1)}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}fr-core-1:If identityReliability status = 'VALI', then at least Patient.identifier[INS-NIR] or Patient.identifier[INS-NIA] or Patient.identifier[INS-NIR-TEST] or Patient.identifier[INS-NIR-DEMO] SHALL be present {(extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-identity-reliability').extension('identityStatus').value.exists(code = 'VALI')) implies (identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.8' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.9' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.10' and use = 'official').exists() or identifier.where(system = 'urn:oid:1.2.250.1.213.1.4.11' and use = 'official').exists())}fr-core-2:If identityReliability status = 'VALI', then only one identifier of type official SHALL be present {(extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-identity-reliability').extension('identityStatus').value.exists(code = 'VALI')) implies (identifier.where(use = 'official').count() = 1)}fr-core-3:If identityReliability status = 'VALI', then the municipality of birth COG code cannot be 99999 because this code cannot be sent by the INSI online service. {(extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-identity-reliability').extension('identityStatus').value.exists(code = 'VALI')) implies extension('http://hl7.org/fhir/StructureDefinition/patient-birthPlace').value.extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-address-insee-code').value.code != '99999')}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>

</xml_diff>